<commit_message>
contrasenasGrupos 0.2 TomSelect y Doc
Agregado TomSelect para el multiselect
Casi completada Documentación.
</commit_message>
<xml_diff>
--- a/doc/ES.xlsx
+++ b/doc/ES.xlsx
@@ -37,6 +37,21 @@
     <t xml:space="preserve">Tipo</t>
   </si>
   <si>
+    <t xml:space="preserve">CRUD usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite al usuario crear y/o modificar su cuenta
+En el sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Correo
+- Contraseña
+- Políticas de privacidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login</t>
   </si>
   <si>
@@ -48,9 +63,6 @@
 - Contraseña</t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
     <t xml:space="preserve">Logout</t>
   </si>
   <si>
@@ -60,42 +72,42 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">CRUD usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permite al usuario crear y/o modificar su cuenta
-En el sistema.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Nombre completo
-- Fecha de nacimiento
-- Correo
-- Contraseña</t>
+    <t xml:space="preserve">CRUD Grupos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite al usuario crear grupos donde pueda 
+Almacenar sus contraseñas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Nombre
+- Descripción</t>
   </si>
   <si>
     <t xml:space="preserve">CRUD contraseña</t>
   </si>
   <si>
     <t xml:space="preserve">Permite al usuario crear, editar o “borrar” una
-Contraseña de un servicio, dispositivos, etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Contraseña
-- Iconografia
+Contraseña de un servicio, dispositivos, etc.
+También se le permite almacenarla en una
+O varias carpetas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Nombre de usuario – Correo
+- Contraseña
 - Descripción</t>
   </si>
   <si>
     <t xml:space="preserve">Contraseñas usuarios</t>
   </si>
   <si>
-    <t xml:space="preserve">Muestra las contraseñas del usuario, ocultas o
-No, con un icono y descripción para saber a que
-Pertenece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Estado (oculta o no)
-- Contraseña
-- Iconografía
+    <t xml:space="preserve">Muestra las contraseñas del usuario, ocultas
+Con múltiples botones para eliminar, borrar y
+Copiar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Nombre usuario – Correo
+- Contraseña (Oculta y
+Encriptada)
 - Descripción</t>
   </si>
   <si>
@@ -110,19 +122,7 @@
 Usuario</t>
   </si>
   <si>
-    <t xml:space="preserve">- Tema
-- Color A
-- Color B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pagar Premium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistema de pago que da beneficios al 
-Usuario (API)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Datos tarjeta</t>
+    <t xml:space="preserve">- Oscuro o claro</t>
   </si>
 </sst>
 </file>
@@ -210,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -251,12 +251,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -336,10 +340,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="S19" activeCellId="0" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,174 +389,174 @@
         <v>7</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="12"/>
+      <c r="I9" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="4"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="4"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="11.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -563,7 +567,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -573,40 +577,40 @@
       <c r="I15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="5"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -616,73 +620,115 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="7"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="34">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:F3"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:F8"/>
-    <mergeCell ref="G5:H8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:F11"/>
-    <mergeCell ref="G9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:F15"/>
-    <mergeCell ref="G12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:F18"/>
-    <mergeCell ref="G16:H18"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:F20"/>
-    <mergeCell ref="G19:H20"/>
-    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:F5"/>
+    <mergeCell ref="G2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:F12"/>
+    <mergeCell ref="G9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:F16"/>
+    <mergeCell ref="G13:H16"/>
+    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:F20"/>
+    <mergeCell ref="G17:H20"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:F23"/>
+    <mergeCell ref="G21:H23"/>
+    <mergeCell ref="I21:I23"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>